<commit_message>
full code. All scripts and graph code
</commit_message>
<xml_diff>
--- a/Makita/doc2vec/output/tables/metrics/metrics_sim_van_de_Schoot_2018.xlsx
+++ b/Makita/doc2vec/output/tables/metrics/metrics_sim_van_de_Schoot_2018.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices-my.sharepoint.com/personal/s_d_willems_students_uu_nl/Documents/Thesis/ASReview/Simulation_study_PTSD/Makita/doc2vec/output/tables/metrics/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_186960F7F613C806CD13805A23B6CC3274520185" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DC675CA-AAFC-4F43-8E56-FE242F8CB966}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>file_name</t>
   </si>
@@ -28,6 +22,18 @@
     <t>recall_0.1</t>
   </si>
   <si>
+    <t>recall_0.25</t>
+  </si>
+  <si>
+    <t>recall_0.5</t>
+  </si>
+  <si>
+    <t>recall_0.75</t>
+  </si>
+  <si>
+    <t>recall_0.9</t>
+  </si>
+  <si>
     <t>wss_0.95</t>
   </si>
   <si>
@@ -37,38 +43,14 @@
     <t>atd</t>
   </si>
   <si>
-    <t>Add Absolute Minimum - Logistic</t>
-  </si>
-  <si>
-    <t>CDF - Logistic</t>
-  </si>
-  <si>
-    <t>Min-Max - Logistic</t>
-  </si>
-  <si>
-    <t>Sigmoid - Logistic</t>
-  </si>
-  <si>
-    <t>Doc2Vec - Logistic (baseline)</t>
-  </si>
-  <si>
-    <t>Add Absolute Minimum - NB</t>
-  </si>
-  <si>
-    <t>CDF - NB</t>
-  </si>
-  <si>
-    <t>Min-Max - NB</t>
-  </si>
-  <si>
-    <t>Sigmoid - NB</t>
+    <t>metrics_sim_van_de_Schoot_2018_logistic_doc2vec_default_max_double.json</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,21 +113,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -183,7 +157,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -217,7 +191,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -252,10 +225,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -428,19 +400,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="28.54296875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -456,192 +423,52 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2">
-        <v>0.94594594594594594</v>
+        <v>0.9459459459459459</v>
       </c>
       <c r="D2">
-        <v>0.8432408630559225</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>0.83783783783783783</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>193.027027027027</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>0.94594594594594594</v>
-      </c>
-      <c r="D3">
-        <v>0.83465433729634519</v>
-      </c>
-      <c r="E3">
-        <v>0.83783783783783783</v>
-      </c>
-      <c r="F3">
-        <v>213.94594594594591</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>0.91891891891891897</v>
-      </c>
-      <c r="D4">
-        <v>0.83245266402465878</v>
-      </c>
-      <c r="E4">
-        <v>0.81081081081081086</v>
-      </c>
-      <c r="F4">
-        <v>277.13513513513522</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>0.91891891891891897</v>
-      </c>
-      <c r="D5">
-        <v>0.83179216204315276</v>
-      </c>
-      <c r="E5">
-        <v>0.81081081081081086</v>
-      </c>
-      <c r="F5">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6">
-        <v>0.89189189189189189</v>
-      </c>
-      <c r="D6">
-        <v>0.83135182738881552</v>
-      </c>
-      <c r="E6">
-        <v>0.78378378378378377</v>
-      </c>
-      <c r="F6">
-        <v>190.81081081081081</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>0.91891891891891897</v>
-      </c>
-      <c r="D7">
-        <v>0.8276089828269485</v>
-      </c>
-      <c r="E7">
-        <v>0.81081081081081086</v>
-      </c>
-      <c r="F7">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8">
-        <v>0.91891891891891897</v>
-      </c>
-      <c r="D8">
-        <v>0.81836195508586529</v>
-      </c>
-      <c r="E8">
-        <v>0.81081081081081086</v>
-      </c>
-      <c r="F8">
-        <v>234.29729729729729</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9">
-        <v>0.89189189189189189</v>
-      </c>
-      <c r="D9">
-        <v>0.81219726992514307</v>
-      </c>
-      <c r="E9">
-        <v>0.78378378378378377</v>
-      </c>
-      <c r="F9">
-        <v>234.59459459459461</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10">
-        <v>0.86486486486486491</v>
-      </c>
-      <c r="D10">
-        <v>0.80405107881990312</v>
-      </c>
-      <c r="E10">
-        <v>0.7567567567567568</v>
-      </c>
-      <c r="F10">
-        <v>249.08108108108109</v>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0.8487450462351387</v>
+      </c>
+      <c r="I2">
+        <v>0.8378378378378378</v>
+      </c>
+      <c r="J2">
+        <v>228.2162162162162</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F10">
-    <sortCondition descending="1" ref="D1:D10"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>